<commit_message>
Refactor: Single-page dashboard with improved formatting
- Restructured app to single-page interface with sidebar uploads
- Updated File 2 structure to handle last fortnight data (engagement, post_count, day_won, rank)
- Added Last Fortnight Day Won and Last Fortnight Rank columns to dashboard
- Formatted engagement values in millions with M suffix (e.g., 0.45M)
- Rounded percentages to 0 decimal places with % sign
- Fixed copy-paste formatting for percentages (now pastes as '42%' not '41.873422')
- Added interactive tooltips for all column headers
- Updated column order per spec: Follower, Page, Post, Engagement, Rank, Day Won, % changes, Last Fortnight metrics
- Fixed 'cannot insert Name (Profile)' aggregation error
- Maintained data precision in Excel/CSV exports
</commit_message>
<xml_diff>
--- a/exampleupload2.xlsx
+++ b/exampleupload2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amartyaanand/Documents/inclusive/smreportauto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amartyaanand/Documents/inclusive/smauto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD37CB4A-6098-A34A-BD34-FD061CDD78C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{406AFB32-17BE-214D-A325-CE016D289FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="8700" windowWidth="27640" windowHeight="15600" xr2:uid="{5FF12EE4-648E-DD46-BA16-8C05F6238F45}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{5FF12EE4-648E-DD46-BA16-8C05F6238F45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name (Profile)</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>R.J.D - राष्ट्रीय जनता दल</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Days Won</t>
   </si>
 </sst>
 </file>
@@ -447,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EAD520B-A2FC-1445-8C07-2DD21E488960}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +471,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -476,8 +488,14 @@
       <c r="C2" s="2">
         <v>584427</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -487,8 +505,14 @@
       <c r="C3" s="2">
         <v>1287930</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -498,8 +522,14 @@
       <c r="C4" s="2">
         <v>2339960</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -509,8 +539,14 @@
       <c r="C5" s="2">
         <v>584566</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -520,8 +556,14 @@
       <c r="C6" s="2">
         <v>401046</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -530,6 +572,12 @@
       </c>
       <c r="C7" s="2">
         <v>1230241</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>